<commit_message>
styling new 6 oct
</commit_message>
<xml_diff>
--- a/Main Website/media/L_T/TC Incentive/TC Performance L_T.xlsx
+++ b/Main Website/media/L_T/TC Incentive/TC Performance L_T.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,41 +579,6 @@
           <t>INCENTIVE</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>EMPLOYEE_ID</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>MANAGER_ID</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>DESIGNATION</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>STAFF</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>EMPLOYEE_STATUS</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>PROCESS</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>DEPARTMENT</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -630,7 +595,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3741096</v>
+        <v>3741096.000000004</v>
       </c>
       <c r="E2" t="n">
         <v>170</v>
@@ -660,7 +625,7 @@
         <v>1055962.39</v>
       </c>
       <c r="N2" t="n">
-        <v>2664495.91</v>
+        <v>2664495.910000002</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -706,41 +671,6 @@
       </c>
       <c r="AC2" t="n">
         <v>2000</v>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>O286</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>O162</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>TC</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>OFFICE</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>ACTIVE</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>L&amp;T</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>TW</t>
-        </is>
       </c>
     </row>
     <row r="3">
@@ -758,7 +688,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>5761856.23</v>
+        <v>5761856.230000002</v>
       </c>
       <c r="E3" t="n">
         <v>208</v>
@@ -785,10 +715,10 @@
         <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>2171842.19</v>
+        <v>2171842.189999999</v>
       </c>
       <c r="N3" t="n">
-        <v>3487508.66</v>
+        <v>3487508.659999999</v>
       </c>
       <c r="O3" t="n">
         <v>70728.56</v>
@@ -834,41 +764,6 @@
       </c>
       <c r="AC3" t="n">
         <v>1000</v>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>O283</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>P226</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>TC</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>OFFICE</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>ACTIVE</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>L&amp;T</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>TW</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>